<commit_message>
pharmacy steps removed done for CPR
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_Provider.xlsx
+++ b/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_Provider.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27465" windowHeight="13230"/>
+    <workbookView windowWidth="28680" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458">
   <si>
     <t>Step No</t>
   </si>
@@ -792,45 +792,6 @@
   </si>
   <si>
     <t>Diagnosis date selected</t>
-  </si>
-  <si>
-    <t>MEDICATION_NAME</t>
-  </si>
-  <si>
-    <t>Type Medication name</t>
-  </si>
-  <si>
-    <t>Medication name entered</t>
-  </si>
-  <si>
-    <t>Select Medication name</t>
-  </si>
-  <si>
-    <t>Medication name selected</t>
-  </si>
-  <si>
-    <t>DOSAGE</t>
-  </si>
-  <si>
-    <t>TestDosage</t>
-  </si>
-  <si>
-    <t>Enter Dosage</t>
-  </si>
-  <si>
-    <t>Dosage entered</t>
-  </si>
-  <si>
-    <t>FREQUENCY</t>
-  </si>
-  <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>Enter frequency</t>
-  </si>
-  <si>
-    <t>Frequency entered</t>
   </si>
   <si>
     <t>SELF_LASTPAGE</t>
@@ -1455,8 +1416,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1483,8 +1444,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1498,31 +1506,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1536,6 +1543,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1543,54 +1558,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1604,26 +1573,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1648,13 +1609,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,43 +1633,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1720,19 +1657,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1744,13 +1681,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1762,13 +1699,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1786,7 +1741,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1798,13 +1753,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1817,6 +1766,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1881,41 +1842,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1949,8 +1875,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1978,10 +1928,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1999,130 +1960,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2593,10 +2554,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H200"/>
+  <dimension ref="A1:H195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -5165,7 +5126,7 @@
       <c r="H119" s="8"/>
     </row>
     <row r="120" spans="1:8">
-      <c r="A120" s="7">
+      <c r="A120" s="8">
         <v>119</v>
       </c>
       <c r="B120" s="7" t="s">
@@ -5190,1626 +5151,1520 @@
       <c r="A121" s="8">
         <v>120</v>
       </c>
-      <c r="B121" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F121" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="G121" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="H121" s="8"/>
+      <c r="B121" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H121" s="7"/>
     </row>
     <row r="122" spans="1:8">
-      <c r="A122" s="7">
+      <c r="A122" s="8">
         <v>121</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="B122" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7">
-        <v>5</v>
-      </c>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-      <c r="H122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8">
+        <v>4</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H122" s="8"/>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" s="8">
         <v>122</v>
       </c>
-      <c r="B123" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="G123" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="H123" s="8"/>
+      <c r="B123" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H123" s="7"/>
     </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="7">
+      <c r="A124" s="8">
         <v>123</v>
       </c>
-      <c r="B124" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="E124" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="F124" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="G124" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="H124" s="7"/>
+      <c r="B124" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8">
+        <v>1</v>
+      </c>
+      <c r="F124" s="8"/>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" s="8">
         <v>124</v>
       </c>
-      <c r="B125" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="F125" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="G125" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="H125" s="8"/>
+      <c r="B125" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="7"/>
+      <c r="H125" s="7"/>
     </row>
     <row r="126" spans="1:8">
-      <c r="A126" s="7">
+      <c r="A126" s="8">
         <v>125</v>
       </c>
-      <c r="B126" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E126" s="7"/>
-      <c r="F126" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G126" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H126" s="7"/>
+      <c r="B126" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8">
+        <v>1</v>
+      </c>
+      <c r="F126" s="8"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="8">
         <v>126</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="B127" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H127" s="7"/>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="8">
+        <v>127</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8">
-        <v>4</v>
-      </c>
-      <c r="F127" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H127" s="8"/>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="7">
-        <v>127</v>
-      </c>
-      <c r="B128" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="E128" s="7"/>
-      <c r="F128" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="G128" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="H128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8">
+        <v>3</v>
+      </c>
+      <c r="F128" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G128" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="H128" s="8"/>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" s="8">
         <v>128</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8">
-        <v>1</v>
-      </c>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
+      <c r="B129" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H129" s="7"/>
     </row>
     <row r="130" spans="1:8">
-      <c r="A130" s="7">
+      <c r="A130" s="8">
         <v>129</v>
       </c>
-      <c r="B130" s="7" t="s">
+      <c r="B130" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C130" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D130" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
-      <c r="H130" s="7"/>
+      <c r="C130" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G130" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H130" s="8"/>
     </row>
     <row r="131" spans="1:8">
       <c r="A131" s="8">
         <v>130</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="B131" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8">
-        <v>1</v>
-      </c>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7">
+        <v>2</v>
+      </c>
+      <c r="F131" s="7"/>
+      <c r="G131" s="7"/>
+      <c r="H131" s="7"/>
     </row>
     <row r="132" spans="1:8">
-      <c r="A132" s="7">
+      <c r="A132" s="8">
         <v>131</v>
       </c>
-      <c r="B132" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D132" s="7" t="s">
+      <c r="B132" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E132" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="F132" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7" t="s">
+      <c r="G132" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="G132" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="H132" s="7"/>
+      <c r="H132" s="8"/>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" s="8">
         <v>132</v>
       </c>
-      <c r="B133" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8">
-        <v>3</v>
-      </c>
-      <c r="F133" s="8" t="s">
+      <c r="B133" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F133" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="G133" s="8" t="s">
+      <c r="G133" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="H133" s="8"/>
+      <c r="H133" s="7"/>
     </row>
     <row r="134" spans="1:8">
-      <c r="A134" s="7">
+      <c r="A134" s="8">
         <v>133</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D134" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="E134" s="7"/>
-      <c r="F134" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="G134" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="H134" s="7"/>
+      <c r="B134" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E134" s="8">
+        <v>9889656446</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G134" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H134" s="8"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="8">
         <v>134</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C135" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D135" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E135" s="8"/>
-      <c r="F135" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="G135" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="H135" s="8"/>
+      <c r="C135" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="H135" s="7"/>
     </row>
     <row r="136" spans="1:8">
-      <c r="A136" s="7">
+      <c r="A136" s="8">
         <v>135</v>
       </c>
-      <c r="B136" s="7" t="s">
+      <c r="B136" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7">
-        <v>2</v>
-      </c>
-      <c r="F136" s="7"/>
-      <c r="G136" s="7"/>
-      <c r="H136" s="7"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8">
+        <v>4</v>
+      </c>
+      <c r="F136" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G136" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H136" s="8"/>
     </row>
     <row r="137" spans="1:8">
       <c r="A137" s="8">
         <v>136</v>
       </c>
-      <c r="B137" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D137" s="8" t="s">
+      <c r="B137" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G137" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="E137" s="8" t="s">
+      <c r="H137" s="7"/>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="8">
+        <v>137</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D138" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="F137" s="8" t="s">
+      <c r="E138" s="8"/>
+      <c r="F138" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="G137" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="H137" s="8"/>
-    </row>
-    <row r="138" spans="1:8">
-      <c r="A138" s="7">
-        <v>137</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="H138" s="7"/>
+      <c r="G138" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H138" s="8"/>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" s="8">
         <v>138</v>
       </c>
-      <c r="B139" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C139" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D139" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E139" s="8">
-        <v>9889656446</v>
-      </c>
-      <c r="F139" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G139" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H139" s="8"/>
+      <c r="B139" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H139" s="7"/>
     </row>
     <row r="140" spans="1:8">
-      <c r="A140" s="7">
+      <c r="A140" s="8">
         <v>139</v>
       </c>
-      <c r="B140" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H140" s="7"/>
+      <c r="B140" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="G140" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H140" s="8"/>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" s="8">
         <v>140</v>
       </c>
-      <c r="B141" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8">
-        <v>4</v>
-      </c>
-      <c r="F141" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G141" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H141" s="8"/>
+      <c r="B141" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H141" s="7"/>
     </row>
     <row r="142" spans="1:8">
-      <c r="A142" s="7">
+      <c r="A142" s="8">
         <v>141</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="B142" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C142" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D142" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="G142" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="H142" s="7"/>
+      <c r="G142" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H142" s="8"/>
     </row>
     <row r="143" spans="1:8">
       <c r="A143" s="8">
         <v>142</v>
       </c>
-      <c r="B143" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D143" s="8" t="s">
+      <c r="B143" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H143" s="7"/>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" s="8">
+        <v>143</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E144" s="8"/>
+      <c r="F144" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="E143" s="8"/>
-      <c r="F143" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="G143" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="H143" s="8"/>
-    </row>
-    <row r="144" spans="1:8">
-      <c r="A144" s="7">
-        <v>143</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D144" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="G144" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="H144" s="7"/>
+      <c r="G144" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H144" s="8"/>
     </row>
     <row r="145" spans="1:8">
       <c r="A145" s="8">
         <v>144</v>
       </c>
-      <c r="B145" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C145" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D145" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E145" s="8"/>
-      <c r="F145" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="G145" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="H145" s="8"/>
+      <c r="B145" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="H145" s="7"/>
     </row>
     <row r="146" spans="1:8">
-      <c r="A146" s="7">
+      <c r="A146" s="8">
         <v>145</v>
       </c>
-      <c r="B146" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="G146" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="H146" s="7"/>
+      <c r="B146" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8">
+        <v>5</v>
+      </c>
+      <c r="F146" s="8"/>
+      <c r="G146" s="8"/>
+      <c r="H146" s="8"/>
     </row>
     <row r="147" spans="1:8">
       <c r="A147" s="8">
         <v>146</v>
       </c>
-      <c r="B147" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D147" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="G147" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="H147" s="8"/>
+      <c r="B147" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H147" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="148" spans="1:8">
-      <c r="A148" s="7">
+      <c r="A148" s="8">
         <v>147</v>
       </c>
-      <c r="B148" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D148" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="G148" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="H148" s="7"/>
+      <c r="B148" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G148" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H148" s="8"/>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" s="8">
         <v>148</v>
       </c>
-      <c r="B149" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C149" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D149" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="E149" s="8"/>
-      <c r="F149" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="G149" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="H149" s="8"/>
+      <c r="B149" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7">
+        <v>5</v>
+      </c>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
+      <c r="H149" s="7"/>
     </row>
     <row r="150" spans="1:8">
-      <c r="A150" s="7">
+      <c r="A150" s="8">
         <v>149</v>
       </c>
-      <c r="B150" s="7" t="s">
+      <c r="B150" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C150" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D150" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="G150" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="H150" s="7"/>
+      <c r="C150" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E150" s="8"/>
+      <c r="F150" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G150" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H150" s="8"/>
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="8">
         <v>150</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="H151" s="7"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" s="8">
+        <v>151</v>
+      </c>
+      <c r="B152" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8">
-        <v>5</v>
-      </c>
-      <c r="F151" s="8"/>
-      <c r="G151" s="8"/>
-      <c r="H151" s="8"/>
-    </row>
-    <row r="152" spans="1:8">
-      <c r="A152" s="7">
-        <v>151</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G152" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H152" s="7">
-        <v>3</v>
-      </c>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8">
+        <v>20</v>
+      </c>
+      <c r="F152" s="8"/>
+      <c r="G152" s="8"/>
+      <c r="H152" s="8"/>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" s="8">
         <v>152</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="B153" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C153" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D153" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E153" s="8"/>
-      <c r="F153" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G153" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H153" s="8"/>
+      <c r="C153" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="H153" s="7"/>
     </row>
     <row r="154" spans="1:8">
-      <c r="A154" s="7">
+      <c r="A154" s="8">
         <v>153</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7">
-        <v>5</v>
-      </c>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-      <c r="H154" s="7"/>
+      <c r="B154" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F154" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="G154" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="H154" s="8"/>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" s="8">
         <v>154</v>
       </c>
-      <c r="B155" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D155" s="8" t="s">
+      <c r="B155" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D155" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="E155" s="8"/>
-      <c r="F155" s="8" t="s">
+      <c r="E155" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="G155" s="8" t="s">
+      <c r="F155" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H155" s="8"/>
+      <c r="G155" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="H155" s="7"/>
     </row>
     <row r="156" spans="1:8">
-      <c r="A156" s="7">
+      <c r="A156" s="8">
         <v>155</v>
       </c>
-      <c r="B156" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D156" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7" t="s">
+      <c r="B156" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="G156" s="7" t="s">
+      <c r="C156" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D156" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="H156" s="7"/>
+      <c r="E156" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="F156" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="G156" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="H156" s="8"/>
     </row>
     <row r="157" spans="1:8">
       <c r="A157" s="8">
         <v>156</v>
       </c>
-      <c r="B157" s="8" t="s">
+      <c r="B157" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E157" s="7"/>
+      <c r="F157" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="H157" s="7"/>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" s="8">
+        <v>157</v>
+      </c>
+      <c r="B158" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="E157" s="8">
-        <v>20</v>
-      </c>
-      <c r="F157" s="8"/>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-    </row>
-    <row r="158" spans="1:8">
-      <c r="A158" s="7">
-        <v>157</v>
-      </c>
-      <c r="B158" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="E158" s="7"/>
-      <c r="F158" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="G158" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="H158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8">
+        <v>20</v>
+      </c>
+      <c r="F158" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H158" s="8"/>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="8">
         <v>158</v>
       </c>
-      <c r="B159" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C159" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D159" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="F159" s="8" t="s">
+      <c r="B159" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="G159" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="H159" s="8"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
+      <c r="G159" s="7"/>
+      <c r="H159" s="7"/>
     </row>
     <row r="160" spans="1:8">
-      <c r="A160" s="7">
+      <c r="A160" s="8">
         <v>159</v>
       </c>
-      <c r="B160" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D160" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="E160" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="F160" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="G160" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="H160" s="7"/>
+      <c r="B160" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8">
+        <v>10</v>
+      </c>
+      <c r="F160" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G160" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H160" s="8"/>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="8">
         <v>160</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="F161" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="G161" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="H161" s="8"/>
+      <c r="B161" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D161" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="G161" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="H161" s="7"/>
     </row>
     <row r="162" spans="1:8">
-      <c r="A162" s="7">
+      <c r="A162" s="8">
         <v>161</v>
       </c>
-      <c r="B162" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D162" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E162" s="7"/>
-      <c r="F162" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="G162" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="H162" s="7"/>
+      <c r="B162" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8">
+        <v>5</v>
+      </c>
+      <c r="F162" s="8"/>
+      <c r="G162" s="8"/>
+      <c r="H162" s="8"/>
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="8">
         <v>162</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="B163" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D163" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
+      <c r="H163" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164" s="8">
+        <v>163</v>
+      </c>
+      <c r="B164" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-      <c r="E163" s="8">
-        <v>20</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G163" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H163" s="8"/>
-    </row>
-    <row r="164" spans="1:8">
-      <c r="A164" s="7">
-        <v>163</v>
-      </c>
-      <c r="B164" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="7"/>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-      <c r="H164" s="7"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8">
+        <v>1</v>
+      </c>
+      <c r="F164" s="8"/>
+      <c r="G164" s="8"/>
+      <c r="H164" s="8"/>
     </row>
     <row r="165" spans="1:8">
       <c r="A165" s="8">
         <v>164</v>
       </c>
-      <c r="B165" s="8" t="s">
+      <c r="B165" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E165" s="7"/>
+      <c r="F165" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G165" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H165" s="7"/>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166" s="8">
+        <v>165</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C165" s="8"/>
-      <c r="D165" s="8"/>
-      <c r="E165" s="8">
-        <v>10</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G165" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H165" s="8"/>
-    </row>
-    <row r="166" spans="1:8">
-      <c r="A166" s="7">
-        <v>165</v>
-      </c>
-      <c r="B166" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="E166" s="7"/>
-      <c r="F166" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="G166" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="H166" s="7"/>
+      <c r="C166" s="8"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="8">
+        <v>5</v>
+      </c>
+      <c r="F166" s="8"/>
+      <c r="G166" s="8"/>
+      <c r="H166" s="8"/>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="8">
         <v>166</v>
       </c>
-      <c r="B167" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
-      <c r="E167" s="8">
-        <v>5</v>
-      </c>
-      <c r="F167" s="8"/>
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
+      <c r="B167" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="E167" s="7"/>
+      <c r="F167" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G167" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="H167" s="7"/>
     </row>
     <row r="168" spans="1:8">
-      <c r="A168" s="7">
+      <c r="A168" s="8">
         <v>167</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C168" s="7" t="s">
+      <c r="B168" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C168" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D168" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="E168" s="7"/>
-      <c r="F168" s="7"/>
-      <c r="G168" s="7"/>
-      <c r="H168" s="7">
-        <v>3</v>
-      </c>
+      <c r="D168" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E168" s="8"/>
+      <c r="F168" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G168" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="H168" s="8"/>
     </row>
     <row r="169" spans="1:8">
       <c r="A169" s="8">
         <v>168</v>
       </c>
-      <c r="B169" s="8" t="s">
+      <c r="B169" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C169" s="8"/>
-      <c r="D169" s="8"/>
-      <c r="E169" s="8">
-        <v>1</v>
-      </c>
-      <c r="F169" s="8"/>
-      <c r="G169" s="8"/>
-      <c r="H169" s="8"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7">
+        <v>5</v>
+      </c>
+      <c r="F169" s="7"/>
+      <c r="G169" s="7"/>
+      <c r="H169" s="7"/>
     </row>
     <row r="170" spans="1:8">
-      <c r="A170" s="7">
+      <c r="A170" s="8">
         <v>169</v>
       </c>
-      <c r="B170" s="7" t="s">
+      <c r="B170" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C170" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D170" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E170" s="7"/>
-      <c r="F170" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G170" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H170" s="7"/>
+      <c r="C170" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D170" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E170" s="8"/>
+      <c r="F170" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="G170" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="H170" s="8"/>
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="8">
         <v>170</v>
       </c>
-      <c r="B171" s="8" t="s">
+      <c r="B171" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C171" s="8"/>
-      <c r="D171" s="8"/>
-      <c r="E171" s="8">
+      <c r="C171" s="7"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7">
         <v>5</v>
       </c>
-      <c r="F171" s="8"/>
-      <c r="G171" s="8"/>
-      <c r="H171" s="8"/>
+      <c r="F171" s="7"/>
+      <c r="G171" s="7"/>
+      <c r="H171" s="7"/>
     </row>
     <row r="172" spans="1:8">
-      <c r="A172" s="7">
+      <c r="A172" s="8">
         <v>171</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D172" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="E172" s="7"/>
-      <c r="F172" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G172" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="H172" s="7"/>
+      <c r="B172" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="F172" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G172" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="H172" s="8"/>
     </row>
     <row r="173" spans="1:8">
       <c r="A173" s="8">
         <v>172</v>
       </c>
-      <c r="B173" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D173" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E173" s="8"/>
-      <c r="F173" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="G173" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="H173" s="8"/>
+      <c r="B173" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" s="7"/>
+      <c r="D173" s="7"/>
+      <c r="E173" s="7">
+        <v>5</v>
+      </c>
+      <c r="F173" s="7"/>
+      <c r="G173" s="7"/>
+      <c r="H173" s="7"/>
     </row>
     <row r="174" spans="1:8">
-      <c r="A174" s="7">
+      <c r="A174" s="8">
         <v>173</v>
       </c>
-      <c r="B174" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C174" s="7"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="7">
-        <v>5</v>
-      </c>
-      <c r="F174" s="7"/>
-      <c r="G174" s="7"/>
-      <c r="H174" s="7"/>
+      <c r="B174" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+      <c r="E174" s="8"/>
+      <c r="F174" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="G174" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="H174" s="8"/>
     </row>
     <row r="175" spans="1:8">
       <c r="A175" s="8">
         <v>174</v>
       </c>
-      <c r="B175" s="8" t="s">
+      <c r="B175" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C175" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D175" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="E175" s="8"/>
-      <c r="F175" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="G175" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="H175" s="8"/>
+      <c r="C175" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="E175" s="7"/>
+      <c r="F175" s="7"/>
+      <c r="G175" s="7"/>
+      <c r="H175" s="7"/>
     </row>
     <row r="176" spans="1:8">
-      <c r="A176" s="7">
+      <c r="A176" s="8">
         <v>175</v>
       </c>
-      <c r="B176" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C176" s="7"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7">
-        <v>5</v>
-      </c>
-      <c r="F176" s="7"/>
-      <c r="G176" s="7"/>
-      <c r="H176" s="7"/>
+      <c r="B176" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D176" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E176" s="8"/>
+      <c r="F176" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G176" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H176" s="8"/>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="8">
         <v>176</v>
       </c>
-      <c r="B177" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C177" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D177" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="E177" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="F177" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="G177" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="H177" s="8"/>
+      <c r="B177" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7"/>
+      <c r="H177" s="7"/>
     </row>
     <row r="178" spans="1:8">
-      <c r="A178" s="7">
+      <c r="A178" s="8">
         <v>177</v>
       </c>
-      <c r="B178" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C178" s="7"/>
-      <c r="D178" s="7"/>
-      <c r="E178" s="7">
-        <v>5</v>
-      </c>
-      <c r="F178" s="7"/>
-      <c r="G178" s="7"/>
-      <c r="H178" s="7"/>
+      <c r="B178" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D178" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="E178" s="8"/>
+      <c r="F178" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G178" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H178" s="8"/>
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="8">
         <v>178</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
-      <c r="E179" s="8"/>
-      <c r="F179" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="G179" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="H179" s="8"/>
+      <c r="B179" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E179" s="7">
+        <v>200</v>
+      </c>
+      <c r="F179" s="7"/>
+      <c r="G179" s="7"/>
+      <c r="H179" s="7"/>
     </row>
     <row r="180" spans="1:8">
-      <c r="A180" s="7">
+      <c r="A180" s="8">
         <v>179</v>
       </c>
-      <c r="B180" s="7" t="s">
+      <c r="B180" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C180" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D180" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="E180" s="7"/>
-      <c r="F180" s="7"/>
-      <c r="G180" s="7"/>
-      <c r="H180" s="7"/>
+      <c r="C180" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E180" s="8"/>
+      <c r="F180" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G180" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H180" s="8"/>
     </row>
     <row r="181" spans="1:8">
       <c r="A181" s="8">
         <v>180</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C181" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D181" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="E181" s="8"/>
-      <c r="F181" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G181" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H181" s="8"/>
+      <c r="B181" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7">
+        <v>3</v>
+      </c>
+      <c r="F181" s="7"/>
+      <c r="G181" s="7"/>
+      <c r="H181" s="7"/>
     </row>
     <row r="182" spans="1:8">
-      <c r="A182" s="7">
+      <c r="A182" s="8">
         <v>181</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C182" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="E182" s="7"/>
-      <c r="F182" s="7"/>
-      <c r="G182" s="7"/>
-      <c r="H182" s="7"/>
+      <c r="B182" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E182" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F182" s="8"/>
+      <c r="G182" s="8"/>
+      <c r="H182" s="8"/>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" s="8">
         <v>182</v>
       </c>
-      <c r="B183" s="8" t="s">
+      <c r="B183" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E183" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F183" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="G183" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="H183" s="7"/>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" s="8">
+        <v>183</v>
+      </c>
+      <c r="B184" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C183" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D183" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="E183" s="8"/>
-      <c r="F183" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G183" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H183" s="8"/>
-    </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="7">
-        <v>183</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C184" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D184" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="E184" s="7">
-        <v>200</v>
-      </c>
-      <c r="F184" s="7"/>
-      <c r="G184" s="7"/>
-      <c r="H184" s="7"/>
+      <c r="C184" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E184" s="8"/>
+      <c r="F184" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G184" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H184" s="8"/>
     </row>
     <row r="185" spans="1:8">
       <c r="A185" s="8">
         <v>184</v>
       </c>
-      <c r="B185" s="8" t="s">
+      <c r="B185" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7">
+        <v>2</v>
+      </c>
+      <c r="F185" s="7"/>
+      <c r="G185" s="7"/>
+      <c r="H185" s="7"/>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" s="8">
+        <v>185</v>
+      </c>
+      <c r="B186" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C185" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D185" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="E185" s="8"/>
-      <c r="F185" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G185" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H185" s="8"/>
-    </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="7">
-        <v>185</v>
-      </c>
-      <c r="B186" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C186" s="7"/>
-      <c r="D186" s="7"/>
-      <c r="E186" s="7">
-        <v>3</v>
-      </c>
-      <c r="F186" s="7"/>
-      <c r="G186" s="7"/>
-      <c r="H186" s="7"/>
+      <c r="C186" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D186" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="E186" s="8"/>
+      <c r="F186" s="8"/>
+      <c r="G186" s="8"/>
+      <c r="H186" s="8"/>
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="8">
         <v>186</v>
       </c>
-      <c r="B187" s="8" t="s">
+      <c r="B187" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C187" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D187" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E187" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="F187" s="8"/>
-      <c r="G187" s="8"/>
-      <c r="H187" s="8"/>
+      <c r="C187" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D187" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="E187" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F187" s="7"/>
+      <c r="G187" s="7"/>
+      <c r="H187" s="7"/>
     </row>
     <row r="188" spans="1:8">
-      <c r="A188" s="7">
+      <c r="A188" s="8">
         <v>187</v>
       </c>
-      <c r="B188" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D188" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="E188" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="G188" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="H188" s="7"/>
+      <c r="B188" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C188" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D188" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="E188" s="8"/>
+      <c r="F188" s="8"/>
+      <c r="G188" s="8"/>
+      <c r="H188" s="8"/>
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="8">
         <v>188</v>
       </c>
-      <c r="B189" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C189" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D189" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="E189" s="8"/>
-      <c r="F189" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G189" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H189" s="8"/>
+      <c r="B189" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189" s="7"/>
+      <c r="D189" s="7"/>
+      <c r="E189" s="7">
+        <v>10</v>
+      </c>
+      <c r="F189" s="7"/>
+      <c r="G189" s="7"/>
+      <c r="H189" s="7"/>
     </row>
     <row r="190" spans="1:8">
-      <c r="A190" s="7">
+      <c r="A190" s="8">
         <v>189</v>
       </c>
-      <c r="B190" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C190" s="7"/>
-      <c r="D190" s="7"/>
-      <c r="E190" s="7">
-        <v>2</v>
-      </c>
-      <c r="F190" s="7"/>
-      <c r="G190" s="7"/>
-      <c r="H190" s="7"/>
+      <c r="B190" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="8"/>
+      <c r="F190" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="G190" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="H190" s="8"/>
     </row>
     <row r="191" spans="1:8">
       <c r="A191" s="8">
         <v>190</v>
       </c>
-      <c r="B191" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D191" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="E191" s="8"/>
-      <c r="F191" s="8"/>
-      <c r="G191" s="8"/>
-      <c r="H191" s="8"/>
+      <c r="B191" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" s="7"/>
+      <c r="D191" s="7"/>
+      <c r="E191" s="7">
+        <v>10</v>
+      </c>
+      <c r="F191" s="7"/>
+      <c r="G191" s="7"/>
+      <c r="H191" s="7"/>
     </row>
     <row r="192" spans="1:8">
-      <c r="A192" s="7">
+      <c r="A192" s="8">
         <v>191</v>
       </c>
-      <c r="B192" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D192" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="E192" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
-      <c r="H192" s="7"/>
+      <c r="B192" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D192" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E192" s="8"/>
+      <c r="F192" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="G192" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="H192" s="8"/>
     </row>
     <row r="193" spans="1:8">
       <c r="A193" s="8">
         <v>192</v>
       </c>
-      <c r="B193" s="8" t="s">
+      <c r="B193" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="E193" s="7"/>
+      <c r="F193" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="G193" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="H193" s="7"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="8">
+        <v>193</v>
+      </c>
+      <c r="B194" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C193" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D193" s="8" t="s">
+      <c r="C194" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D194" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E194" s="8"/>
+      <c r="F194" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="G194" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="E193" s="8"/>
-      <c r="F193" s="8"/>
-      <c r="G193" s="8"/>
-      <c r="H193" s="8"/>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="7">
-        <v>193</v>
-      </c>
-      <c r="B194" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C194" s="7"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7">
-        <v>10</v>
-      </c>
-      <c r="F194" s="7"/>
-      <c r="G194" s="7"/>
-      <c r="H194" s="7"/>
+      <c r="H194" s="8"/>
     </row>
     <row r="195" spans="1:8">
       <c r="A195" s="8">
         <v>194</v>
       </c>
-      <c r="B195" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="C195" s="8"/>
-      <c r="D195" s="8"/>
-      <c r="E195" s="8"/>
-      <c r="F195" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="G195" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="H195" s="8"/>
-    </row>
-    <row r="196" spans="1:8">
-      <c r="A196" s="7">
-        <v>195</v>
-      </c>
-      <c r="B196" s="7" t="s">
+      <c r="B195" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C196" s="7"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7">
-        <v>10</v>
-      </c>
-      <c r="F196" s="7"/>
-      <c r="G196" s="7"/>
-      <c r="H196" s="7"/>
-    </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="8">
-        <v>196</v>
-      </c>
-      <c r="B197" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="C197" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D197" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="E197" s="8"/>
-      <c r="F197" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="G197" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="H197" s="8"/>
-    </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="7">
-        <v>197</v>
-      </c>
-      <c r="B198" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D198" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="E198" s="7"/>
-      <c r="F198" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="G198" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="H198" s="7"/>
-    </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="8">
-        <v>198</v>
-      </c>
-      <c r="B199" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C199" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D199" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="E199" s="8"/>
-      <c r="F199" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="G199" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="H199" s="8"/>
-    </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="7">
-        <v>199</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C200" s="7"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7">
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7">
         <v>4</v>
       </c>
-      <c r="F200" s="7"/>
-      <c r="G200" s="7"/>
-      <c r="H200" s="7"/>
+      <c r="F195" s="7"/>
+      <c r="G195" s="7"/>
+      <c r="H195" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>[1]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 C10 C11 C12 C13 C152 B153 C153 B154 C154 B4:B13 B14:B15 C7:C9 C14:C15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 C10 C11 C12 C13 C147 B148 C148 B149 C149 B4:B13 B14:B15 C7:C9 C14:C15">
       <formula1>[6]DataList!#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44 C56 C114 C27:C33">
@@ -6821,16 +6676,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C91 B100 C100 B78:B99 B101:B112 C78:C79 C89:C90 C92:C95 C96:C99 C101:C106 C107:C112">
       <formula1>[7]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122 B133 B134 B152 C168 B169 C169 C171 B1:B3 B16:B36 B37:B77 B115:B121 B123:B131 B136:B151 B155:B168 B170:B172 B199:B200 C2:C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128 B129 B147 C163 B164 C164 C166 B1:B3 B16:B36 B37:B77 B115:B120 B121:B126 B131:B146 B150:B163 B165:B167 B194:B195 C2:C3">
       <formula1/>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C170 C16:C26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C165 C16:C26">
       <formula1>[2]DataList!#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B113:B114">
       <formula1>[8]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B173:B176 B177:B198">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B168:B171 B172:B193">
       <formula1>[5]DataList!#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6861,7 +6716,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -6869,20 +6724,20 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="C3" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -6893,20 +6748,20 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="C6" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -6914,47 +6769,47 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="C8" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="C10" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="C11" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -6964,12 +6819,12 @@
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="3:3">
@@ -6979,55 +6834,55 @@
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="2" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="3:3">
@@ -7037,152 +6892,152 @@
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" spans="3:3">
@@ -7192,204 +7047,204 @@
     </row>
     <row r="60" spans="3:3">
       <c r="C60" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="2" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="2" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="2" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="2" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="3" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="3:3">
@@ -7404,12 +7259,12 @@
     </row>
     <row r="100" spans="3:3">
       <c r="C100" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes CPR and LLS files create provider state
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_Provider.xlsx
+++ b/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_Provider.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28680" windowHeight="13650"/>
+    <workbookView windowWidth="28680" windowHeight="13230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398">
   <si>
     <t>Step No</t>
   </si>
@@ -335,108 +335,108 @@
     <t>add 2 entered</t>
   </si>
   <si>
+    <t>SelectByIndex</t>
+  </si>
+  <si>
     <t>CONTACT_STATE</t>
   </si>
   <si>
+    <t>Select state</t>
+  </si>
+  <si>
+    <t>State selected</t>
+  </si>
+  <si>
+    <t>CONTACT_CITY</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Enter CIty</t>
+  </si>
+  <si>
+    <t>City entered</t>
+  </si>
+  <si>
+    <t>CONTACT_ZIPCODE</t>
+  </si>
+  <si>
+    <t>APP_COUNTRY</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Enter Country</t>
+  </si>
+  <si>
+    <t>Coutry entered</t>
+  </si>
+  <si>
+    <t>CONTACT_PHONE_TYPE</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>CONTACT_PNONE_NUMBER</t>
+  </si>
+  <si>
+    <t>CONTACT_SEQUENCE</t>
+  </si>
+  <si>
+    <t>APP_AUTHORIZE_PERSON</t>
+  </si>
+  <si>
+    <t>APP_AUTHORIZE_FNAME</t>
+  </si>
+  <si>
+    <t>TestingBab</t>
+  </si>
+  <si>
+    <t>Enter First  name</t>
+  </si>
+  <si>
+    <t>APP_AUTHORIZE_LNAME</t>
+  </si>
+  <si>
+    <t>bab</t>
+  </si>
+  <si>
+    <t>Enter Last name</t>
+  </si>
+  <si>
+    <t>APP_AUTHO_RELATIONSHIP</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Select Relationship</t>
+  </si>
+  <si>
+    <t>Relationship selected</t>
+  </si>
+  <si>
+    <t>APP_AUTHO_ADDRESS1</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Address </t>
+  </si>
+  <si>
+    <t>Address entered</t>
+  </si>
+  <si>
+    <t>APP_AUTHO_STATE</t>
+  </si>
+  <si>
     <t>California</t>
   </si>
   <si>
-    <t>Select state</t>
-  </si>
-  <si>
-    <t>State selected</t>
-  </si>
-  <si>
-    <t>CONTACT_CITY</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Enter CIty</t>
-  </si>
-  <si>
-    <t>City entered</t>
-  </si>
-  <si>
-    <t>CONTACT_ZIPCODE</t>
-  </si>
-  <si>
-    <t>APP_COUNTRY</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Enter Country</t>
-  </si>
-  <si>
-    <t>Coutry entered</t>
-  </si>
-  <si>
-    <t>CONTACT_PHONE_TYPE</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>CONTACT_PNONE_NUMBER</t>
-  </si>
-  <si>
-    <t>SelectByIndex</t>
-  </si>
-  <si>
-    <t>CONTACT_SEQUENCE</t>
-  </si>
-  <si>
-    <t>APP_AUTHORIZE_PERSON</t>
-  </si>
-  <si>
-    <t>APP_AUTHORIZE_FNAME</t>
-  </si>
-  <si>
-    <t>TestingBab</t>
-  </si>
-  <si>
-    <t>Enter First  name</t>
-  </si>
-  <si>
-    <t>APP_AUTHORIZE_LNAME</t>
-  </si>
-  <si>
-    <t>bab</t>
-  </si>
-  <si>
-    <t>Enter Last name</t>
-  </si>
-  <si>
-    <t>APP_AUTHO_RELATIONSHIP</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Select Relationship</t>
-  </si>
-  <si>
-    <t>Relationship selected</t>
-  </si>
-  <si>
-    <t>APP_AUTHO_ADDRESS1</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter Address </t>
-  </si>
-  <si>
-    <t>Address entered</t>
-  </si>
-  <si>
-    <t>APP_AUTHO_STATE</t>
-  </si>
-  <si>
     <t>Select State</t>
   </si>
   <si>
@@ -632,9 +632,6 @@
     <t>SEARCH_PROV_STATE</t>
   </si>
   <si>
-    <t>Alabama</t>
-  </si>
-  <si>
     <t>Select State from the search popup</t>
   </si>
   <si>
@@ -723,9 +720,6 @@
   </si>
   <si>
     <t>ADD_PROV_PATIENT_STATE</t>
-  </si>
-  <si>
-    <t>Alaska</t>
   </si>
   <si>
     <t>ADD_PROV_CITY</t>
@@ -1240,10 +1234,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1270,6 +1264,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1278,15 +1308,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1309,7 +1332,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1318,6 +1356,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1339,15 +1385,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1363,52 +1403,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1435,7 +1429,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1447,7 +1507,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1459,19 +1543,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,7 +1573,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1495,132 +1609,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1679,13 +1673,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4" tint="0.399975585192419"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.399975585192419"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1695,6 +1693,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1738,21 +1745,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1778,19 +1770,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1808,134 +1791,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1945,7 +1928,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2405,8 +2387,8 @@
   <sheetPr/>
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -3215,16 +3197,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="7" t="s">
         <v>101</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>102</v>
@@ -3351,13 +3333,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="E44" s="7">
         <v>1</v>
@@ -3419,7 +3401,7 @@
         <v>20</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
@@ -3437,13 +3419,13 @@
         <v>15</v>
       </c>
       <c r="D48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>28</v>
@@ -3461,13 +3443,13 @@
         <v>15</v>
       </c>
       <c r="D49" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="F49" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>32</v>
@@ -3485,16 +3467,16 @@
         <v>20</v>
       </c>
       <c r="D50" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="H50" s="7"/>
     </row>
@@ -3509,16 +3491,16 @@
         <v>15</v>
       </c>
       <c r="D51" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="F51" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="G51" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="H51" s="8"/>
     </row>
@@ -3533,10 +3515,10 @@
         <v>20</v>
       </c>
       <c r="D52" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>134</v>
@@ -3746,8 +3728,8 @@
       <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>116</v>
+      <c r="B62" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>20</v>
@@ -3792,8 +3774,8 @@
       <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>116</v>
+      <c r="B64" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>20</v>
@@ -4243,7 +4225,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>20</v>
@@ -4251,11 +4233,11 @@
       <c r="D85" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E85" s="8">
+        <v>1</v>
+      </c>
+      <c r="F85" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="G85" s="8" t="s">
         <v>103</v>
@@ -4273,11 +4255,11 @@
         <v>15</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E86" s="7"/>
       <c r="F86" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>32</v>
@@ -4295,11 +4277,11 @@
         <v>15</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G87" s="8" t="s">
         <v>180</v>
@@ -4317,14 +4299,14 @@
         <v>15</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G88" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="H88" s="7"/>
     </row>
@@ -4359,7 +4341,7 @@
         <v>20</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -4393,11 +4375,11 @@
         <v>20</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>28</v>
@@ -4415,7 +4397,7 @@
         <v>20</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="8" t="s">
@@ -4431,17 +4413,17 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="E94" s="7"/>
       <c r="F94" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>180</v>
@@ -4459,11 +4441,11 @@
         <v>20</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E95" s="8"/>
       <c r="F95" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>180</v>
@@ -4475,17 +4457,17 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E96" s="7"/>
       <c r="F96" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>180</v>
@@ -4503,11 +4485,11 @@
         <v>20</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>35</v>
@@ -4525,11 +4507,11 @@
         <v>20</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>35</v>
@@ -4547,11 +4529,11 @@
         <v>20</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E99" s="8"/>
       <c r="F99" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G99" s="8" t="s">
         <v>35</v>
@@ -4569,16 +4551,16 @@
         <v>20</v>
       </c>
       <c r="D100" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E100" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H100" s="7"/>
     </row>
@@ -4593,16 +4575,16 @@
         <v>20</v>
       </c>
       <c r="D101" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E101" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="F101" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="F101" s="8" t="s">
-        <v>227</v>
-      </c>
       <c r="G101" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H101" s="8"/>
     </row>
@@ -4617,7 +4599,7 @@
         <v>15</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -4629,16 +4611,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
+      </c>
+      <c r="E103" s="8">
+        <v>1</v>
       </c>
       <c r="F103" s="8"/>
       <c r="G103" s="8"/>
@@ -4655,10 +4637,10 @@
         <v>20</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
@@ -4695,7 +4677,7 @@
         <v>15</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E106" s="7">
         <v>9789045678</v>
@@ -4715,7 +4697,7 @@
         <v>15</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E107" s="8">
         <v>21331</v>
@@ -4735,7 +4717,7 @@
         <v>15</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E108" s="7">
         <v>97989898982</v>
@@ -4755,7 +4737,7 @@
         <v>15</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>144</v>
@@ -4775,10 +4757,10 @@
         <v>15</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
@@ -4795,7 +4777,7 @@
         <v>15</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>144</v>
@@ -4815,7 +4797,7 @@
         <v>15</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
@@ -4849,7 +4831,7 @@
         <v>20</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
@@ -4909,16 +4891,16 @@
         <v>20</v>
       </c>
       <c r="D117" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F117" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E117" s="8" t="s">
+      <c r="G117" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G117" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="H117" s="8"/>
     </row>
@@ -4949,10 +4931,10 @@
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G119" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H119" s="8"/>
     </row>
@@ -4967,14 +4949,14 @@
         <v>20</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E120" s="7"/>
       <c r="F120" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H120" s="7"/>
     </row>
@@ -4993,10 +4975,10 @@
       </c>
       <c r="E121" s="8"/>
       <c r="F121" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G121" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H121" s="8"/>
     </row>
@@ -5053,14 +5035,14 @@
         <v>20</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H124" s="7"/>
     </row>
@@ -5075,7 +5057,7 @@
         <v>20</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
@@ -5109,14 +5091,14 @@
         <v>20</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G127" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H127" s="8"/>
     </row>
@@ -5133,10 +5115,10 @@
         <v>5</v>
       </c>
       <c r="F128" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G128" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H128" s="7"/>
     </row>
@@ -5151,14 +5133,14 @@
         <v>20</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E129" s="8"/>
       <c r="F129" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G129" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H129" s="8"/>
     </row>
@@ -5173,14 +5155,14 @@
         <v>20</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E130" s="7"/>
       <c r="F130" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H130" s="7"/>
     </row>
@@ -5211,16 +5193,16 @@
         <v>15</v>
       </c>
       <c r="D132" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F132" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E132" s="7" t="s">
+      <c r="G132" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="F132" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="G132" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="H132" s="7"/>
     </row>
@@ -5235,16 +5217,16 @@
         <v>15</v>
       </c>
       <c r="D133" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G133" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="F133" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="G133" s="8" t="s">
-        <v>272</v>
       </c>
       <c r="H133" s="8"/>
     </row>
@@ -5259,7 +5241,7 @@
         <v>15</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E134" s="7">
         <v>9889656446</v>
@@ -5283,14 +5265,14 @@
         <v>15</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G135" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H135" s="8"/>
     </row>
@@ -5319,20 +5301,20 @@
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E137" s="8"/>
       <c r="F137" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H137" s="8"/>
     </row>
@@ -5341,20 +5323,20 @@
         <v>137</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E138" s="7"/>
       <c r="F138" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H138" s="7"/>
     </row>
@@ -5363,20 +5345,20 @@
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E139" s="8"/>
       <c r="F139" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H139" s="8"/>
     </row>
@@ -5385,20 +5367,20 @@
         <v>139</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E140" s="7"/>
       <c r="F140" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H140" s="7"/>
     </row>
@@ -5407,20 +5389,20 @@
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C141" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E141" s="8"/>
       <c r="F141" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G141" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H141" s="8"/>
     </row>
@@ -5429,20 +5411,20 @@
         <v>141</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E142" s="7"/>
       <c r="F142" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H142" s="7"/>
     </row>
@@ -5451,20 +5433,20 @@
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E143" s="8"/>
       <c r="F143" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G143" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H143" s="8"/>
     </row>
@@ -5473,20 +5455,20 @@
         <v>143</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E144" s="7"/>
       <c r="F144" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H144" s="7"/>
     </row>
@@ -5501,14 +5483,14 @@
         <v>20</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E145" s="8"/>
       <c r="F145" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G145" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H145" s="8"/>
     </row>
@@ -5539,14 +5521,14 @@
         <v>20</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E147" s="8"/>
       <c r="F147" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G147" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H147" s="8"/>
     </row>
@@ -5623,7 +5605,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5631,20 +5613,20 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -5655,20 +5637,20 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -5676,47 +5658,47 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -5726,12 +5708,12 @@
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="3:3">
@@ -5741,55 +5723,55 @@
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="3:3">
@@ -5799,152 +5781,152 @@
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" spans="3:3">
@@ -5954,204 +5936,204 @@
     </row>
     <row r="60" spans="3:3">
       <c r="C60" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="98" spans="3:3">
@@ -6166,12 +6148,12 @@
     </row>
     <row r="100" spans="3:3">
       <c r="C100" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>